<commit_message>
Auto-committed on 2022/05/23 週一 11:49:51.79
</commit_message>
<xml_diff>
--- a/Program/Other/L4321_LNW171E底稿(10909調息檔)機動-地區別調整.xlsx
+++ b/Program/Other/L4321_LNW171E底稿(10909調息檔)機動-地區別調整.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8309DB-F537-4665-9E12-96046D6A46C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="正常件" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">正常件!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">正常件!$A$1:$O$1</definedName>
     <definedName name="_xlnm.Database" localSheetId="0">正常件!$A$1:$M$1</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve"> 目前生效日  </t>
   </si>
@@ -71,18 +70,6 @@
   </si>
   <si>
     <t>繳息迄日</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>擬調</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>下限</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>上限</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
@@ -101,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0000"/>
     <numFmt numFmtId="177" formatCode="#,##0_);[Red]\(#,##0\)"/>
@@ -718,7 +705,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -744,9 +731,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1072,11 +1056,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1090,12 +1074,11 @@
     <col min="12" max="12" width="10.109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="25.44140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" style="3" customWidth="1"/>
-    <col min="15" max="17" width="9" style="1"/>
-    <col min="18" max="18" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="1"/>
+    <col min="15" max="15" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1130,25 +1113,16 @@
         <v>11</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>